<commit_message>
entity has changed cvs added
</commit_message>
<xml_diff>
--- a/upload_files/Efe_Mazlumoglu_CV1__booking_data_engineer_senior.xlsx
+++ b/upload_files/Efe_Mazlumoglu_CV1__booking_data_engineer_senior.xlsx
@@ -187,10 +187,10 @@
     <t>iot : 2</t>
   </si>
   <si>
+    <t>java : 1</t>
+  </si>
+  <si>
     <t>programming : 1</t>
-  </si>
-  <si>
-    <t>java : 1</t>
   </si>
   <si>
     <t>7.407</t>

</xml_diff>